<commit_message>
add testng.xml and other changes
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/userData.xlsx
+++ b/src/main/resources/TestData/userData.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="76">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -113,25 +115,142 @@
     <t xml:space="preserve">demo account</t>
   </si>
   <si>
+    <t xml:space="preserve">zipCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MobNumb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HomeNumb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15112346aru123@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tester2</t>
   </si>
   <si>
+    <t xml:space="preserve">Bhavu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1511113212qw@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tester3</t>
   </si>
   <si>
+    <t xml:space="preserve">Mrs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meghu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1122Meghu12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12!@#qwe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tester4</t>
   </si>
   <si>
+    <t xml:space="preserve">pal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gopal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12gopal@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13!@#qwe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tester5</t>
   </si>
   <si>
-    <t xml:space="preserve">zipCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MobNumb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HomeNumb</t>
+    <t xml:space="preserve">sing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deepika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12ravi@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14!@#qwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tester6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1bhavu12345@gmai.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15!@#qwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tester7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heena12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16!@#qwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tester8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roshan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roshan@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17!@#qwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vasava1234@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arun123@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz@gmail11.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcd12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyx12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arun12@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARUN@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arunvasava@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -168,6 +287,7 @@
       <color rgb="FF871094"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -219,7 +339,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,6 +358,26 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -319,8 +459,8 @@
   </sheetPr>
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,30 +571,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="A8" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -479,30 +597,30 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>36</v>
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="5" t="n">
         <v>12345</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="5" t="n">
         <v>123456789</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="5" t="n">
         <v>987654321</v>
       </c>
     </row>
@@ -515,4 +633,692 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="6" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="22.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="6" width="11.64"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="7" t="n">
+        <v>12345</v>
+      </c>
+      <c r="R2" s="7" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="S2" s="7" t="n">
+        <v>987654321</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <v>12345</v>
+      </c>
+      <c r="R3" s="7" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="S3" s="7" t="n">
+        <v>987654321</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>45678</v>
+      </c>
+      <c r="R4" s="7" t="n">
+        <v>123456790</v>
+      </c>
+      <c r="S4" s="6" t="n">
+        <v>123465789</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="6" t="n">
+        <v>45679</v>
+      </c>
+      <c r="R5" s="7" t="n">
+        <v>123456791</v>
+      </c>
+      <c r="S5" s="6" t="n">
+        <v>123465790</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="6" t="n">
+        <v>45680</v>
+      </c>
+      <c r="R6" s="7" t="n">
+        <v>123456792</v>
+      </c>
+      <c r="S6" s="6" t="n">
+        <v>123465791</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="6" t="n">
+        <v>45681</v>
+      </c>
+      <c r="R7" s="7" t="n">
+        <v>123456793</v>
+      </c>
+      <c r="S7" s="6" t="n">
+        <v>123465792</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="6" t="n">
+        <v>45682</v>
+      </c>
+      <c r="R8" s="7" t="n">
+        <v>123456794</v>
+      </c>
+      <c r="S8" s="6" t="n">
+        <v>123465793</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="6" t="n">
+        <v>45683</v>
+      </c>
+      <c r="R9" s="7" t="n">
+        <v>123456795</v>
+      </c>
+      <c r="S9" s="6" t="n">
+        <v>123465794</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="15112346aru123@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId2" display="12!@qw"/>
+    <hyperlink ref="E3" r:id="rId3" display="1511113212qw@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId4" display="12!@qw"/>
+    <hyperlink ref="E4" r:id="rId5" display="1122Meghu12@gmail.com"/>
+    <hyperlink ref="E5" r:id="rId6" display="12gopal@gmail.com"/>
+    <hyperlink ref="E6" r:id="rId7" display="12ravi@gmail.com"/>
+    <hyperlink ref="E7" r:id="rId8" display="bhavu12345@gmai.com"/>
+    <hyperlink ref="E8" r:id="rId9" display="heena12@gmail.com"/>
+    <hyperlink ref="E9" r:id="rId10" display="roshan@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.84"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="xyz12@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId2" display="vasava1234@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="arun123@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId4" display="xyz@gmail11.com"/>
+    <hyperlink ref="A5" r:id="rId5" display="1234@gmail.com"/>
+    <hyperlink ref="A6" r:id="rId6" display="abcd12@gmail.com"/>
+    <hyperlink ref="A7" r:id="rId7" display="xyx12@gmail.com"/>
+    <hyperlink ref="A8" r:id="rId8" display="Arun12@gmail.com"/>
+    <hyperlink ref="A9" r:id="rId9" display="ARUN@gmail.com"/>
+    <hyperlink ref="A10" r:id="rId10" display="arunvasava@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>